<commit_message>
EKE for Table 2
</commit_message>
<xml_diff>
--- a/Table 2 - Nutricline:MLD/Nutricline-MLD.xlsx
+++ b/Table 2 - Nutricline:MLD/Nutricline-MLD.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25880" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Cruise</t>
   </si>
@@ -297,6 +297,61 @@
   </si>
   <si>
     <t>Check units</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>EKE 157-159W,30-32N</t>
+  </si>
+  <si>
+    <r>
+      <t>EKE (m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cm</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -595,7 +650,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -619,18 +674,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -662,8 +723,11 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -675,6 +739,10 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -686,6 +754,10 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -723,7 +795,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -817,11 +888,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104788600"/>
-        <c:axId val="-2104677704"/>
+        <c:axId val="2131205528"/>
+        <c:axId val="2131211032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104788600"/>
+        <c:axId val="2131205528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="105.0"/>
@@ -850,19 +921,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104677704"/>
+        <c:crossAx val="2131211032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104677704"/>
+        <c:axId val="2131211032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,14 +960,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104788600"/>
+        <c:crossAx val="2131205528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -929,7 +998,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -997,11 +1065,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2104779736"/>
-        <c:axId val="-2104776728"/>
+        <c:axId val="2131236408"/>
+        <c:axId val="2131239352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2104779736"/>
+        <c:axId val="2131236408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104776728"/>
+        <c:crossAx val="2131239352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1018,7 +1086,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2104776728"/>
+        <c:axId val="2131239352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,7 +1097,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104779736"/>
+        <c:crossAx val="2131236408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1076,7 +1144,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1152,11 +1219,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2104751096"/>
-        <c:axId val="-2104748088"/>
+        <c:axId val="2131265224"/>
+        <c:axId val="2131268168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2104751096"/>
+        <c:axId val="2131265224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1165,7 +1232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104748088"/>
+        <c:crossAx val="2131268168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1173,7 +1240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2104748088"/>
+        <c:axId val="2131268168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1184,7 +1251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104751096"/>
+        <c:crossAx val="2131265224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1293,11 +1360,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2108538328"/>
-        <c:axId val="-2108215640"/>
+        <c:axId val="2131311288"/>
+        <c:axId val="2131314312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2108538328"/>
+        <c:axId val="2131311288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1307,12 +1374,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108215640"/>
+        <c:crossAx val="2131314312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2108215640"/>
+        <c:axId val="2131314312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1323,7 +1390,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108538328"/>
+        <c:crossAx val="2131311288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1437,11 +1504,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2108684008"/>
-        <c:axId val="-2107932568"/>
+        <c:axId val="2131339096"/>
+        <c:axId val="2131342216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2108684008"/>
+        <c:axId val="2131339096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,12 +1518,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107932568"/>
+        <c:crossAx val="2131342216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2107932568"/>
+        <c:axId val="2131342216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,7 +1534,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108684008"/>
+        <c:crossAx val="2131339096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1620,16 +1687,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2111,8 +2178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2123,6 +2190,7 @@
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16">
@@ -2143,20 +2211,23 @@
       <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="17" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2172,7 +2243,7 @@
       <c r="D4" s="5">
         <v>38.299379999999999</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="18">
         <f>I14</f>
         <v>0.49698700000000001</v>
       </c>
@@ -2185,8 +2256,11 @@
       <c r="H4" s="5">
         <v>-3.42</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>1.7849999999999999</v>
+      </c>
+      <c r="J4" s="20">
+        <v>188.4</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2202,7 +2276,7 @@
       <c r="D5" s="5">
         <v>28.950901000000002</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="18">
         <f t="shared" ref="E5:E9" si="0">I15</f>
         <v>1.032899</v>
       </c>
@@ -2215,8 +2289,11 @@
       <c r="H5" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>-0.495</v>
+      </c>
+      <c r="J5" s="20">
+        <v>249.5</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2232,7 +2309,7 @@
       <c r="D6" s="5">
         <v>26.087309999999999</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <f t="shared" si="0"/>
         <v>1.0049779999999999</v>
       </c>
@@ -2245,8 +2322,11 @@
       <c r="H6" s="5">
         <v>-0.45</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>-0.27</v>
+      </c>
+      <c r="J6" s="20">
+        <v>263.3</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2262,7 +2342,7 @@
       <c r="D7" s="5">
         <v>33.810867000000002</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="18">
         <f t="shared" si="0"/>
         <v>0.78273099999999995</v>
       </c>
@@ -2275,8 +2355,11 @@
       <c r="H7" s="5">
         <v>0.4</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>-0.74</v>
+      </c>
+      <c r="J7" s="20">
+        <v>236.2</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2292,7 +2375,7 @@
       <c r="D8" s="5">
         <v>94.491940999999997</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="18">
         <f t="shared" si="0"/>
         <v>0.78498500000000004</v>
       </c>
@@ -2305,38 +2388,44 @@
       <c r="H8" s="5">
         <v>4.57</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>-1.57</v>
       </c>
+      <c r="J8" s="20">
+        <v>153.9</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>2011</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>86.919090999999995</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>111.853056</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>56.227001000000001</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="19">
         <f t="shared" si="0"/>
         <v>0.63125500000000001</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>49.657685999999998</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>36.500247000000002</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>2.23</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>-0.76</v>
+      </c>
+      <c r="J9" s="21">
+        <v>171.5</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2344,6 +2433,14 @@
         <v>34</v>
       </c>
     </row>
+    <row r="12" spans="1:10">
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="13" spans="1:10">
       <c r="H13" t="s">
         <v>32</v>
@@ -2351,6 +2448,9 @@
       <c r="I13" t="s">
         <v>33</v>
       </c>
+      <c r="J13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
@@ -2383,8 +2483,7 @@
         <v>0.49698700000000001</v>
       </c>
       <c r="J14">
-        <f>I14-H14</f>
-        <v>8.8397000000000003E-2</v>
+        <v>188.4</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2418,8 +2517,7 @@
         <v>1.032899</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15:J19" si="2">I15-H15</f>
-        <v>0.128749</v>
+        <v>249.5</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2453,8 +2551,7 @@
         <v>1.0049779999999999</v>
       </c>
       <c r="J16">
-        <f t="shared" si="2"/>
-        <v>0.1961179999999999</v>
+        <v>263.3</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2488,8 +2585,7 @@
         <v>0.78273099999999995</v>
       </c>
       <c r="J17">
-        <f t="shared" si="2"/>
-        <v>0.15925099999999992</v>
+        <v>236.2</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2523,8 +2619,7 @@
         <v>0.78498500000000004</v>
       </c>
       <c r="J18">
-        <f t="shared" si="2"/>
-        <v>0.17463499999999998</v>
+        <v>153.9</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2558,190 +2653,189 @@
         <v>0.63125500000000001</v>
       </c>
       <c r="J19">
-        <f t="shared" si="2"/>
-        <v>0.14180500000000001</v>
+        <v>171.5</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16" thickBot="1"/>
     <row r="22" spans="1:10" ht="16" thickBot="1">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="12">
         <v>41.8</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="12">
         <v>42.9</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="12">
         <v>38.299999999999997</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="12">
         <v>69.5</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="12">
         <v>33.4</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="12">
         <v>-3.42</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="13">
         <v>1.7849999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="12">
         <v>86.3</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="12">
         <v>98.8</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="12">
         <v>29</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="12">
         <v>87.4</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="12">
         <v>28.7</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="12">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="13">
         <v>-0.495</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="12">
         <v>106.8</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="12">
         <v>126.6</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="12">
         <v>26.1</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="12">
         <v>117.2</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="12">
         <v>29.7</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="12">
         <v>-0.45</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="13">
         <v>-0.27</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="12">
         <v>86.8</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="12">
         <v>116.1</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="12">
         <v>33.799999999999997</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="12">
         <v>66.5</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="12">
         <v>20.399999999999999</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="12">
         <v>0.4</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="13">
         <v>-0.74</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="12">
         <v>102.6</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="12">
         <v>120.2</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="12">
         <v>94.5</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="12">
         <v>87.4</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="12">
         <v>24.3</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="12">
         <v>4.57</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="13">
         <v>-1.57</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16" thickBot="1">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="15">
         <v>86.9</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="15">
         <v>111.9</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="15">
         <v>56.2</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="15">
         <v>49.7</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="15">
         <v>36.5</v>
       </c>
-      <c r="G28" s="17">
+      <c r="G28" s="15">
         <v>2.23</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="16">
         <v>-0.76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New PCA Figure 7
</commit_message>
<xml_diff>
--- a/Table 2 - Nutricline:MLD/Nutricline-MLD.xlsx
+++ b/Table 2 - Nutricline:MLD/Nutricline-MLD.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32640" windowHeight="20560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
     <sheet name="CSV" sheetId="3" r:id="rId3"/>
     <sheet name="princcomp" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
   <si>
     <t>Cruise</t>
   </si>
@@ -79,163 +80,6 @@
   </si>
   <si>
     <t>DCM (m)</t>
-  </si>
-  <si>
-    <r>
-      <t>Table 2. Indicators including the Nutricline (1 µM NO2+NO3), Mixed Layer Depth (m), the depth of the 15°C isotherm (m), and the integrated chl-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> value from the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in-situ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> fluorometer from 10-200m (mg m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) for all transects averaged over 32°-33°N</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Int Chl-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (mg m</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Int Chl-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> (mg m</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>NPI (NDJFM)</t>
@@ -307,6 +151,213 @@
     <t>EKE 157-159W,30-32N</t>
   </si>
   <si>
+    <t>nutricline</t>
+  </si>
+  <si>
+    <t>depth15</t>
+  </si>
+  <si>
+    <t>mld</t>
+  </si>
+  <si>
+    <t>stratindex</t>
+  </si>
+  <si>
+    <t>npindjfm</t>
+  </si>
+  <si>
+    <t>pdofebmar</t>
+  </si>
+  <si>
+    <t>eke</t>
+  </si>
+  <si>
+    <t>Eigenvalues</t>
+  </si>
+  <si>
+    <t>ind = read.csv('Nutricline-MLD.csv')</t>
+  </si>
+  <si>
+    <t>ind.mat = as.matrix(ind)</t>
+  </si>
+  <si>
+    <t>ind.cent = apply(ind.mat,2,scale,center=TRUE,scale=FALSE)</t>
+  </si>
+  <si>
+    <t>Rotation:</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>PC5</t>
+  </si>
+  <si>
+    <t>PC6</t>
+  </si>
+  <si>
+    <t>Loadings</t>
+  </si>
+  <si>
+    <t>E/P</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>80.272953,</t>
+  </si>
+  <si>
+    <t>0.405244,</t>
+  </si>
+  <si>
+    <t>84.397422,</t>
+  </si>
+  <si>
+    <t>123.597410,</t>
+  </si>
+  <si>
+    <t>47.435877,</t>
+  </si>
+  <si>
+    <t>Physical Indicators for PCA</t>
+  </si>
+  <si>
+    <t>Biological Indicators</t>
+  </si>
+  <si>
+    <r>
+      <t>Table 2. Indicators including the Nutricline (1 µM NO2+NO3), Mixed Layer Depth (m), the depth of the 15°C isotherm (m), and the integrated chl-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> value from the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>in-situ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> fluorometer from 10-100m (mg m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>) for all transects averaged over 32°-33°N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Int Chl-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (mg m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Stratification Index (kg m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>-3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>EKE (m</t>
     </r>
@@ -314,21 +365,18 @@
       <rPr>
         <b/>
         <vertAlign val="superscript"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">2 </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>cm</t>
     </r>
@@ -336,57 +384,107 @@
       <rPr>
         <b/>
         <vertAlign val="superscript"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>-2</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
-    <t>nutricline</t>
-  </si>
-  <si>
-    <t>depth15</t>
-  </si>
-  <si>
-    <t>mld</t>
-  </si>
-  <si>
-    <t>stratindex</t>
-  </si>
-  <si>
-    <t>npindjfm</t>
-  </si>
-  <si>
-    <t>pdofebmar</t>
-  </si>
-  <si>
-    <t>eke</t>
-  </si>
-  <si>
-    <t>Eigenvalues</t>
-  </si>
-  <si>
-    <t>ind = read.csv('Nutricline-MLD.csv')</t>
-  </si>
-  <si>
-    <t>ind.mat = as.matrix(ind)</t>
-  </si>
-  <si>
-    <t>ind.cent = apply(ind.mat,2,scale,center=TRUE,scale=FALSE)</t>
+    <r>
+      <t>Int Chl-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (mg m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Surface Chl </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(mg m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>-3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -396,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -436,59 +534,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <vertAlign val="superscript"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
     </font>
     <font>
       <b/>
@@ -505,6 +556,79 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -514,7 +638,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -706,8 +830,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="40">
+  <cellStyleXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -748,64 +894,152 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="33" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="33" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="40">
+  <cellStyles count="76">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -825,6 +1059,24 @@
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -844,6 +1096,24 @@
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="33" builtinId="5"/>
   </cellStyles>
@@ -882,6 +1152,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -975,11 +1246,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2105153160"/>
-        <c:axId val="-2105277784"/>
+        <c:axId val="2120004056"/>
+        <c:axId val="2118965752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2105153160"/>
+        <c:axId val="2120004056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="105.0"/>
@@ -1008,18 +1279,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105277784"/>
+        <c:crossAx val="2118965752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2105277784"/>
+        <c:axId val="2118965752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,13 +1319,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105153160"/>
+        <c:crossAx val="2120004056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1085,6 +1358,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1152,11 +1426,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2105218520"/>
-        <c:axId val="-2105215512"/>
+        <c:axId val="2050953544"/>
+        <c:axId val="2050956536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2105218520"/>
+        <c:axId val="2050953544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1165,7 +1439,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105215512"/>
+        <c:crossAx val="2050956536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1173,7 +1447,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105215512"/>
+        <c:axId val="2050956536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1184,7 +1458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105218520"/>
+        <c:crossAx val="2050953544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1231,6 +1505,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1306,11 +1581,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2104871768"/>
-        <c:axId val="-2104868760"/>
+        <c:axId val="2050985576"/>
+        <c:axId val="2050988520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2104871768"/>
+        <c:axId val="2050985576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,7 +1594,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104868760"/>
+        <c:crossAx val="2050988520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1327,7 +1602,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2104868760"/>
+        <c:axId val="2050988520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,7 +1613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104871768"/>
+        <c:crossAx val="2050985576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1385,7 +1660,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Table 2'!$H$14:$H$19</c:f>
+              <c:f>'Table 2'!$H$30:$H$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1412,7 +1687,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Table 2'!$I$14:$I$19</c:f>
+              <c:f>'Table 2'!$I$30:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1447,11 +1722,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2105539496"/>
-        <c:axId val="-2105536472"/>
+        <c:axId val="2050132920"/>
+        <c:axId val="2050135944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2105539496"/>
+        <c:axId val="2050132920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1461,12 +1736,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105536472"/>
+        <c:crossAx val="2050135944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2105536472"/>
+        <c:axId val="2050135944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1477,13 +1752,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105539496"/>
+        <c:crossAx val="2050132920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1528,7 +1804,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Table 2'!$I$4:$I$9</c:f>
+              <c:f>'Table 2'!$G$5:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1555,7 +1831,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Table 2'!$E$4:$E$9</c:f>
+              <c:f>'Table 2'!$E$5:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1590,11 +1866,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2105511576"/>
-        <c:axId val="-2105508488"/>
+        <c:axId val="2050160776"/>
+        <c:axId val="2050163864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2105511576"/>
+        <c:axId val="2050160776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,12 +1880,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105508488"/>
+        <c:crossAx val="2050163864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2105508488"/>
+        <c:axId val="2050163864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1620,13 +1896,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105511576"/>
+        <c:crossAx val="2050160776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1744,13 +2021,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1774,13 +2051,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2261,820 +2538,1099 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="13"/>
+    <col min="2" max="2" width="12.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="13" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="49"/>
+      <c r="B3" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+    </row>
+    <row r="4" spans="1:12" ht="25">
+      <c r="A4" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="32" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="31">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="G4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4">
+      <c r="H4" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="34">
         <v>1998</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B5" s="35">
         <v>41.808756000000002</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="35">
         <v>42.891060000000003</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D5" s="35">
         <v>38.299379999999999</v>
       </c>
-      <c r="E4" s="18">
-        <f>I14</f>
+      <c r="E5" s="36">
+        <f>I30</f>
         <v>0.49698700000000001</v>
       </c>
-      <c r="F4" s="5">
-        <v>69.517387999999997</v>
-      </c>
-      <c r="G4" s="5">
-        <v>33.415095000000001</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="F5" s="35">
         <v>-3.42</v>
       </c>
-      <c r="I4" s="5">
+      <c r="G5" s="35">
         <v>1.7849999999999999</v>
       </c>
-      <c r="J4" s="20">
+      <c r="H5" s="37">
         <v>188.4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="4">
+    <row r="6" spans="1:12">
+      <c r="A6" s="34">
         <v>1999</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B6" s="35">
         <v>86.306306000000006</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6" s="35">
         <v>98.812477000000001</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D6" s="35">
         <v>28.950901000000002</v>
       </c>
-      <c r="E5" s="18">
-        <f t="shared" ref="E5:E9" si="0">I15</f>
+      <c r="E6" s="36">
+        <f t="shared" ref="E6:E10" si="0">I31</f>
         <v>1.032899</v>
       </c>
-      <c r="F5" s="5">
-        <v>87.389474000000007</v>
-      </c>
-      <c r="G5" s="5">
-        <v>28.698871</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="F6" s="35">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I5" s="5">
+      <c r="G6" s="35">
         <v>-0.495</v>
       </c>
-      <c r="J5" s="20">
+      <c r="H6" s="37">
         <v>249.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="4">
+    <row r="7" spans="1:12">
+      <c r="A7" s="34">
         <v>2000</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B7" s="35">
         <v>106.784712</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="35">
         <v>126.632471</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D7" s="35">
         <v>26.087309999999999</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E7" s="36">
         <f t="shared" si="0"/>
         <v>1.0049779999999999</v>
       </c>
-      <c r="F6" s="5">
-        <v>117.17282</v>
-      </c>
-      <c r="G6" s="5">
-        <v>29.725396</v>
-      </c>
-      <c r="H6" s="5">
+      <c r="F7" s="35">
         <v>-0.45</v>
       </c>
-      <c r="I6" s="5">
+      <c r="G7" s="35">
         <v>-0.27</v>
       </c>
-      <c r="J6" s="20">
+      <c r="H7" s="37">
         <v>263.3</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="4">
+    <row r="8" spans="1:12">
+      <c r="A8" s="34">
         <v>2008</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B8" s="35">
         <v>86.775431999999995</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C8" s="35">
         <v>116.133245</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D8" s="35">
         <v>33.810867000000002</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E8" s="36">
         <f t="shared" si="0"/>
         <v>0.78273099999999995</v>
       </c>
-      <c r="F7" s="5">
-        <v>66.538556</v>
-      </c>
-      <c r="G7" s="5">
-        <v>20.416257999999999</v>
-      </c>
-      <c r="H7" s="5">
+      <c r="F8" s="35">
         <v>0.4</v>
       </c>
-      <c r="I7" s="5">
+      <c r="G8" s="35">
         <v>-0.74</v>
       </c>
-      <c r="J7" s="20">
+      <c r="H8" s="37">
         <v>236.2</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4">
+    <row r="9" spans="1:12">
+      <c r="A9" s="34">
         <v>2009</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B9" s="35">
         <v>102.58216</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="35">
         <v>120.200975</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D9" s="35">
         <v>94.491940999999997</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E9" s="36">
         <f t="shared" si="0"/>
         <v>0.78498500000000004</v>
       </c>
-      <c r="F8" s="5">
-        <v>87.389474000000007</v>
-      </c>
-      <c r="G8" s="5">
-        <v>24.272943000000001</v>
-      </c>
-      <c r="H8" s="5">
+      <c r="F9" s="35">
         <v>4.57</v>
       </c>
-      <c r="I8" s="5">
+      <c r="G9" s="35">
         <v>-1.57</v>
       </c>
-      <c r="J8" s="20">
+      <c r="H9" s="37">
         <v>153.9</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="6">
+    <row r="10" spans="1:12">
+      <c r="A10" s="42">
         <v>2011</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="43">
         <v>86.919090999999995</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C10" s="43">
         <v>111.853056</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10" s="43">
         <v>56.227001000000001</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E10" s="44">
         <f t="shared" si="0"/>
         <v>0.63125500000000001</v>
       </c>
-      <c r="F9" s="7">
-        <v>49.657685999999998</v>
-      </c>
-      <c r="G9" s="7">
-        <v>36.500247000000002</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="F10" s="43">
         <v>2.23</v>
       </c>
-      <c r="I9" s="7">
+      <c r="G10" s="43">
         <v>-0.76</v>
       </c>
-      <c r="J9" s="21">
+      <c r="H10" s="45">
         <v>171.5</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="H12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="H13" t="s">
+    <row r="11" spans="1:12">
+      <c r="A11" s="47"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="35"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="49"/>
+      <c r="B12" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="53"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" ht="25">
+      <c r="A13" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="35"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="34">
+        <v>1998</v>
+      </c>
+      <c r="B14" s="17">
+        <v>69.5</v>
+      </c>
+      <c r="C14" s="35">
+        <v>26.436437000000002</v>
+      </c>
+      <c r="D14" s="39">
+        <v>0.22861699999999999</v>
+      </c>
+      <c r="E14" s="38">
+        <v>7.4128680401116913</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="35"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="34">
+        <v>1999</v>
+      </c>
+      <c r="B15" s="17">
+        <v>87.4</v>
+      </c>
+      <c r="C15" s="35">
+        <v>18.904487</v>
+      </c>
+      <c r="D15" s="39">
+        <v>0.12625400000000001</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="35"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="34">
+        <v>2000</v>
+      </c>
+      <c r="B16" s="17">
+        <v>117.2</v>
+      </c>
+      <c r="C16" s="35">
+        <v>11.582420000000001</v>
+      </c>
+      <c r="D16" s="39">
+        <v>0.106519</v>
+      </c>
+      <c r="E16" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="35"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="34">
+        <v>2008</v>
+      </c>
+      <c r="B17" s="17">
+        <v>66.5</v>
+      </c>
+      <c r="C17" s="35">
+        <v>15.851388999999999</v>
+      </c>
+      <c r="D17" s="41">
+        <v>6.3746999999999998E-2</v>
+      </c>
+      <c r="E17" s="57">
+        <v>0.59517597372125763</v>
+      </c>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="35"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="34">
+        <v>2009</v>
+      </c>
+      <c r="B18" s="17">
+        <v>87.4</v>
+      </c>
+      <c r="C18" s="35">
+        <v>15.538976999999999</v>
+      </c>
+      <c r="D18" s="39">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="E18" s="38">
+        <v>0.48151795220409982</v>
+      </c>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="35"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="42">
+        <v>2011</v>
+      </c>
+      <c r="B19" s="52">
+        <v>49.7</v>
+      </c>
+      <c r="C19" s="43">
+        <v>28.840872000000001</v>
+      </c>
+      <c r="D19" s="44">
+        <v>0.25532199999999999</v>
+      </c>
+      <c r="E19" s="46">
+        <v>0.8002835730200526</v>
+      </c>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="35"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="47"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="35"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="47"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="40"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="14"/>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="22">
+        <v>-0.46836230000000001</v>
+      </c>
+      <c r="C23" s="22">
+        <v>-0.46201059999999999</v>
+      </c>
+      <c r="D23" s="18">
+        <v>-0.2355739</v>
+      </c>
+      <c r="E23" s="18">
+        <v>-0.28217239999999999</v>
+      </c>
+      <c r="F23" s="22">
+        <v>-0.44426520000000003</v>
+      </c>
+      <c r="G23" s="22">
+        <v>0.48419000000000001</v>
+      </c>
+      <c r="H23" s="18">
+        <v>1.5969899999999999E-2</v>
+      </c>
+      <c r="I23" s="14"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="18">
+        <v>-0.16031398999999999</v>
+      </c>
+      <c r="C24" s="18">
+        <v>-0.14747626</v>
+      </c>
+      <c r="D24" s="22">
+        <v>0.52939738000000003</v>
+      </c>
+      <c r="E24" s="22">
+        <v>-0.46592230000000001</v>
+      </c>
+      <c r="F24" s="18">
+        <v>0.25582366000000001</v>
+      </c>
+      <c r="G24" s="18">
+        <v>-5.4510129999999997E-2</v>
+      </c>
+      <c r="H24" s="22">
+        <v>-0.62192274999999997</v>
+      </c>
+      <c r="I24" s="14"/>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="23"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="E26" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="H28" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I28" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="H29" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="J13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14">
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="13">
         <v>1998</v>
       </c>
-      <c r="B14">
+      <c r="B30" s="13">
         <v>41.808756000000002</v>
       </c>
-      <c r="C14">
+      <c r="C30" s="13">
         <v>38.286174000000003</v>
       </c>
-      <c r="D14">
+      <c r="D30" s="13">
         <v>42.891136000000003</v>
       </c>
-      <c r="E14">
+      <c r="E30" s="13">
         <v>69.517387999999997</v>
       </c>
-      <c r="F14">
+      <c r="F30" s="13">
         <v>33.415095000000001</v>
       </c>
-      <c r="G14">
+      <c r="G30" s="13">
         <v>3.143E-3</v>
       </c>
-      <c r="H14">
-        <f>G14*130</f>
+      <c r="H30" s="13">
+        <f>G30*130</f>
         <v>0.40859000000000001</v>
       </c>
-      <c r="I14">
-        <f>F33</f>
+      <c r="I30" s="13">
+        <f>F49</f>
         <v>0.49698700000000001</v>
       </c>
-      <c r="J14">
+      <c r="J30" s="13">
         <v>188.4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15">
+    <row r="31" spans="1:12">
+      <c r="A31" s="13">
         <v>1999</v>
       </c>
-      <c r="B15">
+      <c r="B31" s="13">
         <v>86.306306000000006</v>
       </c>
-      <c r="C15">
+      <c r="C31" s="13">
         <v>28.952216</v>
       </c>
-      <c r="D15">
+      <c r="D31" s="13">
         <v>98.821010999999999</v>
       </c>
-      <c r="E15">
+      <c r="E31" s="13">
         <v>87.389474000000007</v>
       </c>
-      <c r="F15">
+      <c r="F31" s="13">
         <v>28.698871</v>
       </c>
-      <c r="G15">
+      <c r="G31" s="13">
         <v>6.9550000000000002E-3</v>
       </c>
-      <c r="H15">
-        <f t="shared" ref="H15:H19" si="1">G15*130</f>
+      <c r="H31" s="13">
+        <f t="shared" ref="H31:H35" si="1">G31*130</f>
         <v>0.90415000000000001</v>
       </c>
-      <c r="I15">
-        <f>F35</f>
+      <c r="I31" s="13">
+        <f>F51</f>
         <v>1.032899</v>
       </c>
-      <c r="J15">
+      <c r="J31" s="13">
         <v>249.5</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16">
+    <row r="32" spans="1:12">
+      <c r="A32" s="13">
         <v>2000</v>
       </c>
-      <c r="B16">
+      <c r="B32" s="13">
         <v>106.784712</v>
       </c>
-      <c r="C16">
+      <c r="C32" s="13">
         <v>26.076087999999999</v>
       </c>
-      <c r="D16">
+      <c r="D32" s="13">
         <v>126.624956</v>
       </c>
-      <c r="E16">
+      <c r="E32" s="13">
         <v>117.17282</v>
       </c>
-      <c r="F16">
+      <c r="F32" s="13">
         <v>29.725396</v>
       </c>
-      <c r="G16">
+      <c r="G32" s="13">
         <v>6.2220000000000001E-3</v>
       </c>
-      <c r="H16">
+      <c r="H32" s="13">
         <f t="shared" si="1"/>
         <v>0.80886000000000002</v>
       </c>
-      <c r="I16">
-        <f>F37</f>
+      <c r="I32" s="13">
+        <f>F53</f>
         <v>1.0049779999999999</v>
       </c>
-      <c r="J16">
+      <c r="J32" s="13">
         <v>263.3</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
+    <row r="33" spans="1:10">
+      <c r="A33" s="13">
         <v>2008</v>
       </c>
-      <c r="B17">
+      <c r="B33" s="13">
         <v>86.775431999999995</v>
       </c>
-      <c r="C17">
+      <c r="C33" s="13">
         <v>33.813245000000002</v>
       </c>
-      <c r="D17">
+      <c r="D33" s="13">
         <v>116.13805000000001</v>
       </c>
-      <c r="E17">
+      <c r="E33" s="13">
         <v>66.538556</v>
       </c>
-      <c r="F17">
+      <c r="F33" s="13">
         <v>20.416257999999999</v>
       </c>
-      <c r="G17">
+      <c r="G33" s="13">
         <v>4.7959999999999999E-3</v>
       </c>
-      <c r="H17">
+      <c r="H33" s="13">
         <f t="shared" si="1"/>
         <v>0.62348000000000003</v>
       </c>
-      <c r="I17">
-        <f>F39</f>
+      <c r="I33" s="13">
+        <f>F55</f>
         <v>0.78273099999999995</v>
       </c>
-      <c r="J17">
+      <c r="J33" s="13">
         <v>236.2</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
+    <row r="34" spans="1:10">
+      <c r="A34" s="13">
         <v>2009</v>
       </c>
-      <c r="B18">
+      <c r="B34" s="13">
         <v>102.58216</v>
       </c>
-      <c r="C18">
+      <c r="C34" s="13">
         <v>94.475402000000003</v>
       </c>
-      <c r="D18">
+      <c r="D34" s="13">
         <v>120.199269</v>
       </c>
-      <c r="E18">
+      <c r="E34" s="13">
         <v>87.389474000000007</v>
       </c>
-      <c r="F18">
+      <c r="F34" s="13">
         <v>24.272943000000001</v>
       </c>
-      <c r="G18">
+      <c r="G34" s="13">
         <v>4.6950000000000004E-3</v>
       </c>
-      <c r="H18">
+      <c r="H34" s="13">
         <f t="shared" si="1"/>
         <v>0.61035000000000006</v>
       </c>
-      <c r="I18">
-        <f>F41</f>
+      <c r="I34" s="13">
+        <f>F57</f>
         <v>0.78498500000000004</v>
       </c>
-      <c r="J18">
+      <c r="J34" s="13">
         <v>153.9</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19">
+    <row r="35" spans="1:10">
+      <c r="A35" s="13">
         <v>2011</v>
       </c>
-      <c r="B19">
+      <c r="B35" s="13">
         <v>86.919090999999995</v>
       </c>
-      <c r="C19">
+      <c r="C35" s="13">
         <v>56.324672999999997</v>
       </c>
-      <c r="D19">
+      <c r="D35" s="13">
         <v>111.861851</v>
       </c>
-      <c r="E19">
+      <c r="E35" s="13">
         <v>49.657685999999998</v>
       </c>
-      <c r="F19">
+      <c r="F35" s="13">
         <v>36.500247000000002</v>
       </c>
-      <c r="G19">
+      <c r="G35" s="13">
         <v>3.7650000000000001E-3</v>
       </c>
-      <c r="H19">
+      <c r="H35" s="13">
         <f t="shared" si="1"/>
         <v>0.48945</v>
       </c>
-      <c r="I19">
-        <f>F43</f>
+      <c r="I35" s="13">
+        <f>F59</f>
         <v>0.63125500000000001</v>
       </c>
-      <c r="J19">
+      <c r="J35" s="13">
         <v>171.5</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="16" thickBot="1"/>
-    <row r="22" spans="1:10" ht="16" thickBot="1">
-      <c r="A22" s="8" t="s">
+    <row r="37" spans="1:10" ht="16" thickBot="1"/>
+    <row r="38" spans="1:10" ht="16" thickBot="1">
+      <c r="A38" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B38" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C38" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D38" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E38" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="10" t="s">
+      <c r="F38" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="17">
+        <v>41.8</v>
+      </c>
+      <c r="C39" s="17">
+        <v>42.9</v>
+      </c>
+      <c r="D39" s="17">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="E39" s="17">
+        <v>69.5</v>
+      </c>
+      <c r="F39" s="17">
+        <v>33.4</v>
+      </c>
+      <c r="G39" s="17">
+        <v>-3.42</v>
+      </c>
+      <c r="H39" s="28">
+        <v>1.7849999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="17">
+        <v>86.3</v>
+      </c>
+      <c r="C40" s="17">
+        <v>98.8</v>
+      </c>
+      <c r="D40" s="17">
+        <v>29</v>
+      </c>
+      <c r="E40" s="17">
+        <v>87.4</v>
+      </c>
+      <c r="F40" s="17">
+        <v>28.7</v>
+      </c>
+      <c r="G40" s="17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H40" s="28">
+        <v>-0.495</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="17">
+        <v>106.8</v>
+      </c>
+      <c r="C41" s="17">
+        <v>126.6</v>
+      </c>
+      <c r="D41" s="17">
+        <v>26.1</v>
+      </c>
+      <c r="E41" s="17">
+        <v>117.2</v>
+      </c>
+      <c r="F41" s="17">
+        <v>29.7</v>
+      </c>
+      <c r="G41" s="17">
+        <v>-0.45</v>
+      </c>
+      <c r="H41" s="28">
+        <v>-0.27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="17">
+        <v>86.8</v>
+      </c>
+      <c r="C42" s="17">
+        <v>116.1</v>
+      </c>
+      <c r="D42" s="17">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="E42" s="17">
+        <v>66.5</v>
+      </c>
+      <c r="F42" s="17">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="G42" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="H42" s="28">
+        <v>-0.74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="17">
+        <v>102.6</v>
+      </c>
+      <c r="C43" s="17">
+        <v>120.2</v>
+      </c>
+      <c r="D43" s="17">
+        <v>94.5</v>
+      </c>
+      <c r="E43" s="17">
+        <v>87.4</v>
+      </c>
+      <c r="F43" s="17">
+        <v>24.3</v>
+      </c>
+      <c r="G43" s="17">
+        <v>4.57</v>
+      </c>
+      <c r="H43" s="28">
+        <v>-1.57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="16" thickBot="1">
+      <c r="A44" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="19">
+        <v>86.9</v>
+      </c>
+      <c r="C44" s="19">
+        <v>111.9</v>
+      </c>
+      <c r="D44" s="19">
+        <v>56.2</v>
+      </c>
+      <c r="E44" s="19">
+        <v>49.7</v>
+      </c>
+      <c r="F44" s="19">
+        <v>36.5</v>
+      </c>
+      <c r="G44" s="19">
+        <v>2.23</v>
+      </c>
+      <c r="H44" s="30">
+        <v>-0.76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="12">
-        <v>41.8</v>
-      </c>
-      <c r="C23" s="12">
-        <v>42.9</v>
-      </c>
-      <c r="D23" s="12">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="E23" s="12">
-        <v>69.5</v>
-      </c>
-      <c r="F23" s="12">
-        <v>33.4</v>
-      </c>
-      <c r="G23" s="12">
-        <v>-3.42</v>
-      </c>
-      <c r="H23" s="13">
-        <v>1.7849999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="12">
-        <v>86.3</v>
-      </c>
-      <c r="C24" s="12">
-        <v>98.8</v>
-      </c>
-      <c r="D24" s="12">
-        <v>29</v>
-      </c>
-      <c r="E24" s="12">
-        <v>87.4</v>
-      </c>
-      <c r="F24" s="12">
-        <v>28.7</v>
-      </c>
-      <c r="G24" s="12">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H24" s="13">
-        <v>-0.495</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="12">
-        <v>106.8</v>
-      </c>
-      <c r="C25" s="12">
-        <v>126.6</v>
-      </c>
-      <c r="D25" s="12">
-        <v>26.1</v>
-      </c>
-      <c r="E25" s="12">
-        <v>117.2</v>
-      </c>
-      <c r="F25" s="12">
-        <v>29.7</v>
-      </c>
-      <c r="G25" s="12">
-        <v>-0.45</v>
-      </c>
-      <c r="H25" s="13">
-        <v>-0.27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="12">
-        <v>86.8</v>
-      </c>
-      <c r="C26" s="12">
-        <v>116.1</v>
-      </c>
-      <c r="D26" s="12">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="E26" s="12">
-        <v>66.5</v>
-      </c>
-      <c r="F26" s="12">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="G26" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="H26" s="13">
-        <v>-0.74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="12">
-        <v>102.6</v>
-      </c>
-      <c r="C27" s="12">
-        <v>120.2</v>
-      </c>
-      <c r="D27" s="12">
-        <v>94.5</v>
-      </c>
-      <c r="E27" s="12">
-        <v>87.4</v>
-      </c>
-      <c r="F27" s="12">
-        <v>24.3</v>
-      </c>
-      <c r="G27" s="12">
-        <v>4.57</v>
-      </c>
-      <c r="H27" s="13">
-        <v>-1.57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="16" thickBot="1">
-      <c r="A28" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="15">
-        <v>86.9</v>
-      </c>
-      <c r="C28" s="15">
-        <v>111.9</v>
-      </c>
-      <c r="D28" s="15">
-        <v>56.2</v>
-      </c>
-      <c r="E28" s="15">
-        <v>49.7</v>
-      </c>
-      <c r="F28" s="15">
-        <v>36.5</v>
-      </c>
-      <c r="G28" s="15">
-        <v>2.23</v>
-      </c>
-      <c r="H28" s="16">
-        <v>-0.76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" t="s">
+    <row r="49" spans="1:6">
+      <c r="A49" s="13">
+        <v>41.808756000000002</v>
+      </c>
+      <c r="B49" s="13">
+        <v>38.290171999999998</v>
+      </c>
+      <c r="C49" s="13">
+        <v>42.888444</v>
+      </c>
+      <c r="D49" s="13">
+        <v>69.517387999999997</v>
+      </c>
+      <c r="E49" s="13">
+        <v>33.415095000000001</v>
+      </c>
+      <c r="F49" s="13">
+        <v>0.49698700000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="13">
+        <v>86.306306000000006</v>
+      </c>
+      <c r="B51" s="13">
+        <v>28.953703000000001</v>
+      </c>
+      <c r="C51" s="13">
+        <v>98.819947999999997</v>
+      </c>
+      <c r="D51" s="13">
+        <v>87.389474000000007</v>
+      </c>
+      <c r="E51" s="13">
+        <v>28.698871</v>
+      </c>
+      <c r="F51" s="13">
+        <v>1.032899</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="13">
+        <v>106.784712</v>
+      </c>
+      <c r="B53" s="13">
+        <v>26.082858000000002</v>
+      </c>
+      <c r="C53" s="13">
+        <v>126.622759</v>
+      </c>
+      <c r="D53" s="13">
+        <v>117.17282</v>
+      </c>
+      <c r="E53" s="13">
+        <v>29.725396</v>
+      </c>
+      <c r="F53" s="13">
+        <v>1.0049779999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33">
-        <v>41.808756000000002</v>
-      </c>
-      <c r="B33">
-        <v>38.290171999999998</v>
-      </c>
-      <c r="C33">
-        <v>42.888444</v>
-      </c>
-      <c r="D33">
-        <v>69.517387999999997</v>
-      </c>
-      <c r="E33">
-        <v>33.415095000000001</v>
-      </c>
-      <c r="F33">
-        <v>0.49698700000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" s="13">
+        <v>86.775431999999995</v>
+      </c>
+      <c r="B55" s="13">
+        <v>33.787723</v>
+      </c>
+      <c r="C55" s="13">
+        <v>116.12962899999999</v>
+      </c>
+      <c r="D55" s="13">
+        <v>66.538556</v>
+      </c>
+      <c r="E55" s="13">
+        <v>20.416257999999999</v>
+      </c>
+      <c r="F55" s="13">
+        <v>0.78273099999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35">
-        <v>86.306306000000006</v>
-      </c>
-      <c r="B35">
-        <v>28.953703000000001</v>
-      </c>
-      <c r="C35">
-        <v>98.819947999999997</v>
-      </c>
-      <c r="D35">
+    <row r="57" spans="1:6">
+      <c r="A57" s="13">
+        <v>102.58216</v>
+      </c>
+      <c r="B57" s="13">
+        <v>94.472476999999998</v>
+      </c>
+      <c r="C57" s="13">
+        <v>120.199438</v>
+      </c>
+      <c r="D57" s="13">
         <v>87.389474000000007</v>
       </c>
-      <c r="E35">
-        <v>28.698871</v>
-      </c>
-      <c r="F35">
-        <v>1.032899</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
+      <c r="E57" s="13">
+        <v>24.272943000000001</v>
+      </c>
+      <c r="F57" s="13">
+        <v>0.78498500000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37">
-        <v>106.784712</v>
-      </c>
-      <c r="B37">
-        <v>26.082858000000002</v>
-      </c>
-      <c r="C37">
-        <v>126.622759</v>
-      </c>
-      <c r="D37">
-        <v>117.17282</v>
-      </c>
-      <c r="E37">
-        <v>29.725396</v>
-      </c>
-      <c r="F37">
-        <v>1.0049779999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39">
-        <v>86.775431999999995</v>
-      </c>
-      <c r="B39">
-        <v>33.787723</v>
-      </c>
-      <c r="C39">
-        <v>116.12962899999999</v>
-      </c>
-      <c r="D39">
-        <v>66.538556</v>
-      </c>
-      <c r="E39">
-        <v>20.416257999999999</v>
-      </c>
-      <c r="F39">
-        <v>0.78273099999999995</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41">
-        <v>102.58216</v>
-      </c>
-      <c r="B41">
-        <v>94.472476999999998</v>
-      </c>
-      <c r="C41">
-        <v>120.199438</v>
-      </c>
-      <c r="D41">
-        <v>87.389474000000007</v>
-      </c>
-      <c r="E41">
-        <v>24.272943000000001</v>
-      </c>
-      <c r="F41">
-        <v>0.78498500000000004</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43">
+    <row r="59" spans="1:6">
+      <c r="A59" s="13">
         <v>86.919090999999995</v>
       </c>
-      <c r="B43">
+      <c r="B59" s="13">
         <v>56.228071</v>
       </c>
-      <c r="C43">
+      <c r="C59" s="13">
         <v>111.84829999999999</v>
       </c>
-      <c r="D43">
+      <c r="D59" s="13">
         <v>49.657685999999998</v>
       </c>
-      <c r="E43">
+      <c r="E59" s="13">
         <v>36.500247000000002</v>
       </c>
-      <c r="F43">
+      <c r="F59" s="13">
         <v>0.63125500000000001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:D12"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
@@ -3090,170 +3646,170 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="F1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="G1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="25">
+      <c r="A2" s="5">
         <v>41.8</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="5">
         <v>42.9</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="5">
         <v>38.299999999999997</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="6">
         <v>0.5</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="5">
         <v>-3.4</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="5">
         <v>1.8</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="7">
         <v>188.4</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="25">
+      <c r="A3" s="5">
         <v>86.3</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="5">
         <v>98.8</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="5">
         <v>29</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="6">
         <v>1.03</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="5">
         <v>0.6</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="5">
         <v>-0.5</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="7">
         <v>249.5</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="25">
+      <c r="A4" s="5">
         <v>106.8</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="5">
         <v>126.6</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="5">
         <v>26.1</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="5">
         <v>-0.5</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="5">
         <v>-0.3</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="7">
         <v>263.3</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="25">
+      <c r="A5" s="5">
         <v>86.8</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="5">
         <v>116.1</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="5">
         <v>33.799999999999997</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="6">
         <v>0.78</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="5">
         <v>0.4</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="5">
         <v>-0.7</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="7">
         <v>236.2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="25">
+      <c r="A6" s="5">
         <v>102.6</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="5">
         <v>120.2</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="5">
         <v>94.5</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="6">
         <v>0.78</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="5">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="5">
         <v>-1.6</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="7">
         <v>153.9</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="28">
+      <c r="A7" s="8">
         <v>86.9</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="8">
         <v>111.9</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="8">
         <v>56.2</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="9">
         <v>0.63</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="8">
         <v>-0.8</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="10">
         <v>171.5</v>
       </c>
     </row>
@@ -3269,54 +3825,306 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B20" sqref="B20:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="11"/>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="11"/>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="11"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="11"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="11"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="31"/>
-      <c r="E2" t="s">
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="31"/>
-      <c r="E3" t="s">
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="31"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="31"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="31"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="31"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="31"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="31"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="31"/>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>-0.46836230000000001</v>
+      </c>
+      <c r="C12">
+        <v>-0.16031398999999999</v>
+      </c>
+      <c r="D12">
+        <v>0.13693968100000001</v>
+      </c>
+      <c r="E12">
+        <v>0.55066482999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.28111074000000003</v>
+      </c>
+      <c r="G12">
+        <v>0.54037590800000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>-0.46201059999999999</v>
+      </c>
+      <c r="C13">
+        <v>-0.14747626</v>
+      </c>
+      <c r="D13">
+        <v>0.54842859099999997</v>
+      </c>
+      <c r="E13">
+        <v>0.17093679000000001</v>
+      </c>
+      <c r="F13">
+        <v>-7.068576E-2</v>
+      </c>
+      <c r="G13">
+        <v>-0.578863605</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14">
+        <v>-0.2355739</v>
+      </c>
+      <c r="C14">
+        <v>0.52939738000000003</v>
+      </c>
+      <c r="D14">
+        <v>-0.36339936499999997</v>
+      </c>
+      <c r="E14">
+        <v>0.42813479999999998</v>
+      </c>
+      <c r="F14">
+        <v>-0.58316478000000005</v>
+      </c>
+      <c r="G14">
+        <v>-5.1975805999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>-0.28217239999999999</v>
+      </c>
+      <c r="C15">
+        <v>-0.46592230000000001</v>
+      </c>
+      <c r="D15">
+        <v>-0.72019422499999997</v>
+      </c>
+      <c r="E15">
+        <v>4.6675649999999999E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.20117804</v>
+      </c>
+      <c r="G15">
+        <v>-0.37390480199999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16">
+        <v>-0.44426520000000003</v>
+      </c>
+      <c r="C16">
+        <v>0.25582366000000001</v>
+      </c>
+      <c r="D16">
+        <v>-0.15213268999999999</v>
+      </c>
+      <c r="E16">
+        <v>-0.42476458</v>
+      </c>
+      <c r="F16">
+        <v>0.24847111</v>
+      </c>
+      <c r="G16">
+        <v>0.31426820100000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>0.48419000000000001</v>
+      </c>
+      <c r="C17">
+        <v>-5.4510129999999997E-2</v>
+      </c>
+      <c r="D17">
+        <v>-8.0641222999999998E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.54402079000000003</v>
+      </c>
+      <c r="F17">
+        <v>0.28660776999999998</v>
+      </c>
+      <c r="G17">
+        <v>3.5633150000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>1.5969899999999999E-2</v>
+      </c>
+      <c r="C18">
+        <v>-0.62192274999999997</v>
+      </c>
+      <c r="D18">
+        <v>9.3499570000000008E-3</v>
+      </c>
+      <c r="E18">
+        <v>-7.5413949999999993E-2</v>
+      </c>
+      <c r="F18">
+        <v>-0.62573524999999997</v>
+      </c>
+      <c r="G18">
+        <v>0.36280479700000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21">
+        <v>-0.46836230000000001</v>
+      </c>
+      <c r="C21">
+        <v>-0.46201059999999999</v>
+      </c>
+      <c r="D21">
+        <v>-0.2355739</v>
+      </c>
+      <c r="E21">
+        <v>-0.28217239999999999</v>
+      </c>
+      <c r="F21">
+        <v>-0.44426520000000003</v>
+      </c>
+      <c r="G21">
+        <v>0.48419000000000001</v>
+      </c>
+      <c r="H21">
+        <v>1.5969899999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="B22">
+        <v>-0.16031398999999999</v>
+      </c>
+      <c r="C22">
+        <v>-0.14747626</v>
+      </c>
+      <c r="D22">
+        <v>0.52939738000000003</v>
+      </c>
+      <c r="E22">
+        <v>-0.46592230000000001</v>
+      </c>
+      <c r="F22">
+        <v>0.25582366000000001</v>
+      </c>
+      <c r="G22">
+        <v>-5.4510129999999997E-2</v>
+      </c>
+      <c r="H22">
+        <v>-0.62192274999999997</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3327,4 +4135,63 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="16">
+      <c r="B1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2">
+        <v>31.024398000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>